<commit_message>
Finished Ch.4 code and writing
</commit_message>
<xml_diff>
--- a/R_values.xlsx
+++ b/R_values.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davordjekic/Desktop/Bocconi/Thesis/thesis_tex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E4AC0F-95E6-BB42-B929-8232F3182EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45298561-3B4D-394B-8109-D4477DB87039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16400" activeTab="1" xr2:uid="{D00F1173-517D-954F-A331-6A62D90AEC95}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16400" activeTab="4" xr2:uid="{D00F1173-517D-954F-A331-6A62D90AEC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$C$2:$G$56</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="39">
   <si>
     <t>N1</t>
   </si>
@@ -142,6 +146,21 @@
   <si>
     <t>Rho = 2</t>
   </si>
+  <si>
+    <t>Diversification</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Firm Cost</t>
+  </si>
+  <si>
+    <t>Exec Value</t>
+  </si>
+  <si>
+    <t>Deadweight Cost</t>
+  </si>
 </sst>
 </file>
 
@@ -150,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,6 +265,17 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -282,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -320,11 +350,36 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071B629B-07A8-C545-832E-4B712E4A7C39}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H58" sqref="D32:H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -830,10 +885,10 @@
       <c r="H2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="29"/>
+      <c r="L2" s="41"/>
     </row>
     <row r="3" spans="2:12">
       <c r="C3" t="s">
@@ -2019,8 +2074,8 @@
       <c r="F58" s="26">
         <v>2.5</v>
       </c>
-      <c r="G58" s="30"/>
-      <c r="H58" s="31">
+      <c r="G58" s="29"/>
+      <c r="H58" s="30">
         <v>6.0646680993679896</v>
       </c>
       <c r="I58" s="13"/>
@@ -2151,4 +2206,1665 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376436B5-A77A-7647-9B95-B99EA8AF768F}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="C2:G56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" hidden="1">
+      <c r="C3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="32">
+        <v>5.4179298243050704</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" hidden="1">
+      <c r="C4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="32">
+        <v>2.1406800170584201</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" hidden="1">
+      <c r="C5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F5" s="32">
+        <v>-1.1279023259101999</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" hidden="1">
+      <c r="C6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="32">
+        <v>5.4134674158319802</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" hidden="1">
+      <c r="C7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="32">
+        <v>2.1390913737347899</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" hidden="1">
+      <c r="C8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="32">
+        <v>-1.1274802546110001</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" hidden="1">
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="32">
+        <v>5.4102799787651703</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" hidden="1">
+      <c r="C10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="32">
+        <v>2.1379566256857099</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" hidden="1">
+      <c r="C11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="32">
+        <v>-1.1271787760499801</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" hidden="1">
+      <c r="C12" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="32">
+        <v>11.970905444063201</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" hidden="1">
+      <c r="C13" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="32">
+        <v>8.6709856701549093</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" hidden="1">
+      <c r="C14" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="32">
+        <v>5.3775676977417097</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" hidden="1">
+      <c r="C15" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="32">
+        <v>5.5178999324546503</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" hidden="1">
+      <c r="C16" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="32">
+        <v>2.2310907141740102</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" hidden="1">
+      <c r="C17" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F17" s="32">
+        <v>-1.0447778525203399</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" hidden="1">
+      <c r="C18" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F18" s="32">
+        <v>5.5093998440820702</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" hidden="1">
+      <c r="C19" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="32">
+        <v>2.3276265271349499</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" hidden="1">
+      <c r="C20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F20" s="32">
+        <v>-1.04397429202683</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" hidden="1">
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="22">
+        <v>0</v>
+      </c>
+      <c r="E21" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="32">
+        <v>5.5672097291083302</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" hidden="1">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="32">
+        <v>2.3028894772442601</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" hidden="1">
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="22">
+        <v>0</v>
+      </c>
+      <c r="E23" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="F23" s="32">
+        <v>-0.95718675139670495</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" hidden="1">
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="E24" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="32">
+        <v>5.7020205898365601</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" hidden="1">
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="22">
+        <v>2</v>
+      </c>
+      <c r="F25" s="32">
+        <v>2.3514609988561501</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" hidden="1">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="F26" s="32">
+        <v>-0.96960938016884002</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" hidden="1">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F27" s="32">
+        <v>5.6350804180807099</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" hidden="1">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="22">
+        <v>2</v>
+      </c>
+      <c r="F28" s="32">
+        <v>2.3276265271349499</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" hidden="1">
+      <c r="C29" s="25">
+        <v>1</v>
+      </c>
+      <c r="D29" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="E29" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="F29" s="34">
+        <v>-0.96328435100614995</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="32">
+        <v>9.6111270482310402</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" hidden="1">
+      <c r="C31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="32">
+        <v>7.7278885992988897</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" hidden="1">
+      <c r="C32" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F32" s="32">
+        <v>5.8483767290661701</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F33" s="32">
+        <v>9.6030054148038193</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" hidden="1">
+      <c r="C34" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>2</v>
+      </c>
+      <c r="F34" s="32">
+        <v>7.72144844269069</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" hidden="1">
+      <c r="C35" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F35" s="32">
+        <v>5.8436012796467702</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F36" s="32">
+        <v>9.5972042448353001</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" hidden="1">
+      <c r="C37" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2</v>
+      </c>
+      <c r="F37" s="32">
+        <v>7.71684832707047</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" hidden="1">
+      <c r="C38" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F38" s="32">
+        <v>5.8401902402068098</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="C39" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F39" s="32">
+        <v>9.7498868207788707</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" hidden="1">
+      <c r="C40" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2</v>
+      </c>
+      <c r="F40" s="32">
+        <v>7.8548571695294198</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" hidden="1">
+      <c r="C41" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F41" s="32">
+        <v>5.9636881194698299</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="C42" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F42" s="32">
+        <v>9.7220408852833007</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" hidden="1">
+      <c r="C43" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2</v>
+      </c>
+      <c r="F43" s="32">
+        <v>7.8327762633872497</v>
+      </c>
+      <c r="G43" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" hidden="1">
+      <c r="C44" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F44" s="32">
+        <v>5.9473147349525197</v>
+      </c>
+      <c r="G44" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F45" s="32">
+        <v>9.7065709094051194</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" hidden="1">
+      <c r="C46" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2</v>
+      </c>
+      <c r="F46" s="32">
+        <v>7.8205090817343397</v>
+      </c>
+      <c r="G46" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" hidden="1">
+      <c r="C47" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F47" s="32">
+        <v>5.9382183997457201</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7">
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="22">
+        <v>0</v>
+      </c>
+      <c r="E48" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F48" s="32">
+        <v>9.7415007723867895</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" hidden="1">
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="22">
+        <v>0</v>
+      </c>
+      <c r="E49" s="22">
+        <v>2</v>
+      </c>
+      <c r="F49" s="32">
+        <v>7.8649670233949998</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" hidden="1">
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="22">
+        <v>0</v>
+      </c>
+      <c r="E50" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="F50" s="32">
+        <v>5.9921255565465703</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7">
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="E51" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F51" s="32">
+        <v>9.9861059791656803</v>
+      </c>
+      <c r="G51" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" hidden="1">
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+      <c r="D52" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="E52" s="22">
+        <v>2</v>
+      </c>
+      <c r="F52" s="32">
+        <v>8.0591066914486298</v>
+      </c>
+      <c r="G52" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" hidden="1">
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+      <c r="D53" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="E53" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="F53" s="32">
+        <v>6.1363034531753504</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7">
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E54" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F54" s="32">
+        <v>9.8642786689288897</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" hidden="1">
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E55" s="22">
+        <v>2</v>
+      </c>
+      <c r="F55" s="32">
+        <v>7.9625011927758598</v>
+      </c>
+      <c r="G55" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" hidden="1">
+      <c r="C56" s="25">
+        <v>1</v>
+      </c>
+      <c r="D56" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="E56" s="26">
+        <v>2.5</v>
+      </c>
+      <c r="F56" s="34">
+        <v>6.0646680993679896</v>
+      </c>
+      <c r="G56" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C2:G56" xr:uid="{376436B5-A77A-7647-9B95-B99EA8AF768F}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1.5"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="50-50"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8619DE-074F-DB49-89C0-74CD58B4ECAD}">
+  <dimension ref="B2:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="2" spans="2:11">
+      <c r="E2" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="31">
+        <v>0</v>
+      </c>
+      <c r="D4" s="32">
+        <v>14.723398262946899</v>
+      </c>
+      <c r="E4" s="32">
+        <v>5.4179298243050704</v>
+      </c>
+      <c r="F4" s="32">
+        <v>2.1406800170584201</v>
+      </c>
+      <c r="G4" s="32">
+        <v>-1.1279023259101999</v>
+      </c>
+      <c r="H4" s="32">
+        <f>($D4-E4)/$D4</f>
+        <v>0.63201906736844127</v>
+      </c>
+      <c r="I4" s="32">
+        <f t="shared" ref="I4:J19" si="0">($D4-F4)/$D4</f>
+        <v>0.85460693388660935</v>
+      </c>
+      <c r="J4" s="32">
+        <f t="shared" si="0"/>
+        <v>1.0766061140075722</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="32">
+        <v>16.355602566205601</v>
+      </c>
+      <c r="E5" s="32">
+        <v>5.4134674158319802</v>
+      </c>
+      <c r="F5" s="32">
+        <v>2.1390913737347899</v>
+      </c>
+      <c r="G5" s="32">
+        <v>-1.1274802546110001</v>
+      </c>
+      <c r="H5" s="32">
+        <f t="shared" ref="H5:H21" si="1">($D5-E5)/$D5</f>
+        <v>0.66901449250072653</v>
+      </c>
+      <c r="I5" s="32">
+        <f t="shared" si="0"/>
+        <v>0.86921353920921018</v>
+      </c>
+      <c r="J5" s="32">
+        <f t="shared" si="0"/>
+        <v>1.0689354152527912</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="32">
+        <v>17.9878068694644</v>
+      </c>
+      <c r="E6" s="32">
+        <v>5.4102799787651703</v>
+      </c>
+      <c r="F6" s="32">
+        <v>2.1379566256857099</v>
+      </c>
+      <c r="G6" s="32">
+        <v>-1.1271787760499801</v>
+      </c>
+      <c r="H6" s="32">
+        <f t="shared" si="1"/>
+        <v>0.69922514634346489</v>
+      </c>
+      <c r="I6" s="32">
+        <f t="shared" si="0"/>
+        <v>0.88114411939150594</v>
+      </c>
+      <c r="J6" s="32">
+        <f t="shared" si="0"/>
+        <v>1.0626634911209463</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="C7" s="31">
+        <v>0</v>
+      </c>
+      <c r="D7" s="32">
+        <v>13.5802748484204</v>
+      </c>
+      <c r="E7" s="32">
+        <v>5.5332000809876796</v>
+      </c>
+      <c r="F7" s="32">
+        <v>2.2365380355622602</v>
+      </c>
+      <c r="G7" s="21">
+        <v>5.3775676977417097</v>
+      </c>
+      <c r="H7" s="32">
+        <f t="shared" si="1"/>
+        <v>0.5925561048838951</v>
+      </c>
+      <c r="I7" s="32">
+        <f t="shared" si="0"/>
+        <v>0.83530981069780008</v>
+      </c>
+      <c r="J7" s="32">
+        <f t="shared" si="0"/>
+        <v>0.60401628407637087</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="32">
+        <v>15.2124791516791</v>
+      </c>
+      <c r="E8" s="32">
+        <v>5.5178999324546503</v>
+      </c>
+      <c r="F8" s="32">
+        <v>2.2310907141740102</v>
+      </c>
+      <c r="G8" s="32">
+        <v>-1.0447778525203399</v>
+      </c>
+      <c r="H8" s="32">
+        <f t="shared" si="1"/>
+        <v>0.63727806116035968</v>
+      </c>
+      <c r="I8" s="32">
+        <f t="shared" si="0"/>
+        <v>0.85333812510581153</v>
+      </c>
+      <c r="J8" s="32">
+        <f t="shared" si="0"/>
+        <v>1.0686789997937332</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="C9" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="32">
+        <v>16.844683454937901</v>
+      </c>
+      <c r="E9" s="32">
+        <v>5.5093998440820702</v>
+      </c>
+      <c r="F9" s="32">
+        <v>2.3276265271349499</v>
+      </c>
+      <c r="G9" s="32">
+        <v>-1.04397429202683</v>
+      </c>
+      <c r="H9" s="32">
+        <f t="shared" si="1"/>
+        <v>0.67292945226186318</v>
+      </c>
+      <c r="I9" s="32">
+        <f t="shared" si="0"/>
+        <v>0.86181832782066192</v>
+      </c>
+      <c r="J9" s="32">
+        <f t="shared" si="0"/>
+        <v>1.0619764862200956</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="31">
+        <v>1</v>
+      </c>
+      <c r="C10" s="38">
+        <v>0</v>
+      </c>
+      <c r="D10" s="32">
+        <v>12.4371514338939</v>
+      </c>
+      <c r="E10" s="32">
+        <v>5.5672097291083302</v>
+      </c>
+      <c r="F10" s="32">
+        <v>2.3028894772442601</v>
+      </c>
+      <c r="G10" s="32">
+        <v>-0.95718675139670495</v>
+      </c>
+      <c r="H10" s="32">
+        <f t="shared" si="1"/>
+        <v>0.5523726024645409</v>
+      </c>
+      <c r="I10" s="32">
+        <f t="shared" si="0"/>
+        <v>0.81483786786028889</v>
+      </c>
+      <c r="J10" s="32">
+        <f t="shared" si="0"/>
+        <v>1.0769618956948748</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="31">
+        <v>1</v>
+      </c>
+      <c r="C11" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="32">
+        <v>14.0693557371526</v>
+      </c>
+      <c r="E11" s="32">
+        <v>5.7020205898365601</v>
+      </c>
+      <c r="F11" s="32">
+        <v>2.3514609988561501</v>
+      </c>
+      <c r="G11" s="32">
+        <v>-0.96960938016884002</v>
+      </c>
+      <c r="H11" s="32">
+        <f t="shared" si="1"/>
+        <v>0.59472056173976939</v>
+      </c>
+      <c r="I11" s="32">
+        <f t="shared" si="0"/>
+        <v>0.83286647641961997</v>
+      </c>
+      <c r="J11" s="32">
+        <f t="shared" si="0"/>
+        <v>1.0689164023060713</v>
+      </c>
+      <c r="K11" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="39">
+        <v>1</v>
+      </c>
+      <c r="C12" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="34">
+        <v>15.701560040411399</v>
+      </c>
+      <c r="E12" s="34">
+        <v>5.6350804180807099</v>
+      </c>
+      <c r="F12" s="34">
+        <v>2.3276265271349499</v>
+      </c>
+      <c r="G12" s="34">
+        <v>-0.96328435100614995</v>
+      </c>
+      <c r="H12" s="34">
+        <f t="shared" si="1"/>
+        <v>0.64111334137642384</v>
+      </c>
+      <c r="I12" s="34">
+        <f t="shared" si="0"/>
+        <v>0.85175826343724492</v>
+      </c>
+      <c r="J12" s="34">
+        <f t="shared" si="0"/>
+        <v>1.0613495951056409</v>
+      </c>
+      <c r="K12" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="31">
+        <v>0</v>
+      </c>
+      <c r="D13" s="32">
+        <v>14.723398262946899</v>
+      </c>
+      <c r="E13" s="32">
+        <v>9.6111270482310402</v>
+      </c>
+      <c r="F13" s="32">
+        <v>7.7278885992988897</v>
+      </c>
+      <c r="G13" s="32">
+        <v>5.8483767290661701</v>
+      </c>
+      <c r="H13" s="32">
+        <f t="shared" si="1"/>
+        <v>0.34722087410903424</v>
+      </c>
+      <c r="I13" s="32">
+        <f t="shared" si="0"/>
+        <v>0.47512873989512344</v>
+      </c>
+      <c r="J13" s="32">
+        <f t="shared" si="0"/>
+        <v>0.60278349979948087</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="D14" s="32">
+        <v>16.355602566205601</v>
+      </c>
+      <c r="E14" s="32">
+        <v>9.6030054148038193</v>
+      </c>
+      <c r="F14" s="32">
+        <v>7.72144844269069</v>
+      </c>
+      <c r="G14" s="32">
+        <v>5.8436012796467702</v>
+      </c>
+      <c r="H14" s="32">
+        <f t="shared" si="1"/>
+        <v>0.41286141088767864</v>
+      </c>
+      <c r="I14" s="32">
+        <f t="shared" si="0"/>
+        <v>0.52790192770733124</v>
+      </c>
+      <c r="J14" s="32">
+        <f t="shared" si="0"/>
+        <v>0.64271562261356363</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="D15" s="32">
+        <v>17.9878068694644</v>
+      </c>
+      <c r="E15" s="32">
+        <v>9.5972042448353001</v>
+      </c>
+      <c r="F15" s="32">
+        <v>7.71684832707047</v>
+      </c>
+      <c r="G15" s="32">
+        <v>5.8401902402068098</v>
+      </c>
+      <c r="H15" s="32">
+        <f t="shared" si="1"/>
+        <v>0.46646056884637521</v>
+      </c>
+      <c r="I15" s="32">
+        <f t="shared" si="0"/>
+        <v>0.57099559812539591</v>
+      </c>
+      <c r="J15" s="32">
+        <f t="shared" si="0"/>
+        <v>0.67532505309911051</v>
+      </c>
+      <c r="K15" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="C16" s="31">
+        <v>0</v>
+      </c>
+      <c r="D16" s="32">
+        <v>13.5802748484204</v>
+      </c>
+      <c r="E16" s="32">
+        <v>9.7498868207788707</v>
+      </c>
+      <c r="F16" s="32">
+        <v>7.8548571695294198</v>
+      </c>
+      <c r="G16" s="32">
+        <v>5.9636881194698299</v>
+      </c>
+      <c r="H16" s="32">
+        <f t="shared" si="1"/>
+        <v>0.28205526547844972</v>
+      </c>
+      <c r="I16" s="32">
+        <f t="shared" si="0"/>
+        <v>0.42159807093719731</v>
+      </c>
+      <c r="J16" s="32">
+        <f t="shared" si="0"/>
+        <v>0.56085659634764307</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="D17" s="32">
+        <v>15.2124791516791</v>
+      </c>
+      <c r="E17" s="32">
+        <v>9.7220408852833007</v>
+      </c>
+      <c r="F17" s="32">
+        <v>7.8327762633872497</v>
+      </c>
+      <c r="G17" s="32">
+        <v>5.9473147349525197</v>
+      </c>
+      <c r="H17" s="32">
+        <f t="shared" si="1"/>
+        <v>0.36091673235192462</v>
+      </c>
+      <c r="I17" s="32">
+        <f t="shared" si="0"/>
+        <v>0.48510849643316056</v>
+      </c>
+      <c r="J17" s="32">
+        <f t="shared" si="0"/>
+        <v>0.60905026224498882</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="C18" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="32">
+        <v>16.844683454937901</v>
+      </c>
+      <c r="E18" s="32">
+        <v>9.7065709094051194</v>
+      </c>
+      <c r="F18" s="32">
+        <v>7.8205090817343397</v>
+      </c>
+      <c r="G18" s="32">
+        <v>5.9382183997457201</v>
+      </c>
+      <c r="H18" s="32">
+        <f t="shared" si="1"/>
+        <v>0.42376056306598586</v>
+      </c>
+      <c r="I18" s="32">
+        <f t="shared" si="0"/>
+        <v>0.53572834404069414</v>
+      </c>
+      <c r="J18" s="32">
+        <f t="shared" si="0"/>
+        <v>0.64747224751172316</v>
+      </c>
+      <c r="K18" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" s="31">
+        <v>1</v>
+      </c>
+      <c r="C19" s="38">
+        <v>0</v>
+      </c>
+      <c r="D19" s="32">
+        <v>12.4371514338939</v>
+      </c>
+      <c r="E19" s="32">
+        <v>9.7415007723867895</v>
+      </c>
+      <c r="F19" s="32">
+        <v>7.8649670233949998</v>
+      </c>
+      <c r="G19" s="32">
+        <v>5.9921255565465703</v>
+      </c>
+      <c r="H19" s="32">
+        <f t="shared" si="1"/>
+        <v>0.21674180585764083</v>
+      </c>
+      <c r="I19" s="32">
+        <f t="shared" si="0"/>
+        <v>0.36762311971523637</v>
+      </c>
+      <c r="J19" s="32">
+        <f t="shared" si="0"/>
+        <v>0.51820755834678145</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="31">
+        <v>1</v>
+      </c>
+      <c r="C20" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>14.0693557371526</v>
+      </c>
+      <c r="E20" s="32">
+        <v>9.9861059791656803</v>
+      </c>
+      <c r="F20" s="32">
+        <v>8.0591066914486298</v>
+      </c>
+      <c r="G20" s="32">
+        <v>6.1363034531753504</v>
+      </c>
+      <c r="H20" s="32">
+        <f t="shared" si="1"/>
+        <v>0.2902229380130309</v>
+      </c>
+      <c r="I20" s="32">
+        <f t="shared" ref="I20:I21" si="2">($D20-F20)/$D20</f>
+        <v>0.42718722576847312</v>
+      </c>
+      <c r="J20" s="32">
+        <f t="shared" ref="J20:J21" si="3">($D20-G20)/$D20</f>
+        <v>0.56385327318354983</v>
+      </c>
+      <c r="K20" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="39">
+        <v>1</v>
+      </c>
+      <c r="C21" s="40">
+        <v>0.2</v>
+      </c>
+      <c r="D21" s="34">
+        <v>15.701560040411399</v>
+      </c>
+      <c r="E21" s="34">
+        <v>9.8642786689288897</v>
+      </c>
+      <c r="F21" s="34">
+        <v>7.9625011927758598</v>
+      </c>
+      <c r="G21" s="34">
+        <v>6.0646680993679896</v>
+      </c>
+      <c r="H21" s="34">
+        <f t="shared" si="1"/>
+        <v>0.37176442063457321</v>
+      </c>
+      <c r="I21" s="34">
+        <f t="shared" si="2"/>
+        <v>0.49288470876252927</v>
+      </c>
+      <c r="J21" s="34">
+        <f t="shared" si="3"/>
+        <v>0.6137537872823311</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>